<commit_message>
Integração das listas: Inglês, Matemática e Português/Literatura
</commit_message>
<xml_diff>
--- a/ingles_502.xlsx
+++ b/ingles_502.xlsx
@@ -11,18 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <b/>
-        <color rgb="FF000009"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>MARCELO LIMA BEVILAQUA</t>
-    </r>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <r>
       <rPr>
@@ -87,6 +76,116 @@
         <sz val="10.0"/>
       </rPr>
       <t>DANIEL HONORATO</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Times New Roman"/>
+        <b/>
+        <color rgb="FF000009"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>THAIS RODRIGUES OLIVEIRA</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Times New Roman"/>
+        <b/>
+        <color rgb="FF000009"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>EDUARDO RECHDEN OLIVEIRA</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Times New Roman"/>
+        <b/>
+        <color rgb="FF000009"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>FLÁVIA FERNANDES MONTEIRO DANTAS</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Times New Roman"/>
+        <b/>
+        <color rgb="FF000009"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>LIVIA MERCES MARIANO</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Times New Roman"/>
+        <b/>
+        <color rgb="FF000009"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>ELIANE FERREIRA SERAFIM MILITÃO</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Times New Roman"/>
+        <b/>
+        <color rgb="FF000009"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>AMANDA PINTO ALBUQUERQUE PIRES</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Times New Roman"/>
+        <b/>
+        <color rgb="FF000009"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>LILIANE DA SILVA SOUZA</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Times New Roman"/>
+        <b/>
+        <color rgb="FF000009"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>SARA PRISCILA GUSMÃO</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Times New Roman"/>
+        <b/>
+        <color rgb="FF000009"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>EDUARDO MOREIRA DA CUNHA</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Times New Roman"/>
+        <b/>
+        <color rgb="FF000009"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>MARIA MADALENA MENDES FONTES</t>
     </r>
   </si>
   <si>
@@ -97,7 +196,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="###0;###0"/>
+  </numFmts>
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -113,11 +215,6 @@
       <b/>
       <color theme="1"/>
       <name val="Times New Roman"/>
-    </font>
-    <font>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -158,15 +255,15 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="1" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -384,13 +481,12 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="22.0"/>
-    <col customWidth="1" min="2" max="2" width="41.13"/>
+    <col customWidth="1" min="2" max="2" width="29.63"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1">
-        <v>62.0</v>
+        <v>63.0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -398,7 +494,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1">
-        <v>63.0</v>
+        <v>64.0</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>1</v>
@@ -406,7 +502,7 @@
     </row>
     <row r="3">
       <c r="A3" s="1">
-        <v>64.0</v>
+        <v>65.0</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>2</v>
@@ -414,7 +510,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1">
-        <v>65.0</v>
+        <v>66.0</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>3</v>
@@ -422,7 +518,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1">
-        <v>66.0</v>
+        <v>67.0</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>4</v>
@@ -430,7 +526,7 @@
     </row>
     <row r="6">
       <c r="A6" s="1">
-        <v>67.0</v>
+        <v>68.0</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>5</v>
@@ -438,16 +534,88 @@
     </row>
     <row r="7">
       <c r="A7" s="1">
-        <v>68.0</v>
+        <v>69.0</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="3"/>
-      <c r="B8" s="4" t="s">
+      <c r="A8" s="1">
+        <v>70.0</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1">
+        <v>71.0</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1">
+        <v>72.0</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1">
+        <v>73.0</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1">
+        <v>74.0</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1">
+        <v>76.0</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1">
+        <v>77.0</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1">
+        <v>78.0</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="3"/>
+      <c r="B17" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>